<commit_message>
update data; small fixes
</commit_message>
<xml_diff>
--- a/app/data/Visulaization P-Chem Dataset ver2.xlsx
+++ b/app/data/Visulaization P-Chem Dataset ver2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Ptox\chem-viz\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14685"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14690"/>
   </bookViews>
   <sheets>
     <sheet name="default_1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1579" uniqueCount="733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1585" uniqueCount="739">
   <si>
     <t>PREFERRED_NAME</t>
   </si>
@@ -2218,13 +2218,31 @@
   </si>
   <si>
     <t>47.0 °C</t>
+  </si>
+  <si>
+    <t>Bisphenol E</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2081-08-5</t>
+  </si>
+  <si>
+    <t>DTXSID3047891</t>
+  </si>
+  <si>
+    <t>Bisphenol Z</t>
+  </si>
+  <si>
+    <t>843-55-0</t>
+  </si>
+  <si>
+    <t>DTXSID4047963</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -2236,6 +2254,12 @@
       <b/>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2261,12 +2285,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2549,24 +2582,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G263"/>
+  <dimension ref="A1:G265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A251" workbookViewId="0">
+      <selection activeCell="D264" sqref="D264"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="79.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="79.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2589,7 +2622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>680</v>
       </c>
@@ -2612,7 +2645,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>680</v>
       </c>
@@ -2635,7 +2668,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>680</v>
       </c>
@@ -2658,7 +2691,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>443</v>
       </c>
@@ -2681,7 +2714,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>443</v>
       </c>
@@ -2704,7 +2737,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>264</v>
       </c>
@@ -2727,7 +2760,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>264</v>
       </c>
@@ -2750,7 +2783,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>163</v>
       </c>
@@ -2773,7 +2806,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>142</v>
       </c>
@@ -2796,7 +2829,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>349</v>
       </c>
@@ -2819,7 +2852,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>715</v>
       </c>
@@ -2842,7 +2875,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>715</v>
       </c>
@@ -2865,7 +2898,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>630</v>
       </c>
@@ -2888,7 +2921,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>124</v>
       </c>
@@ -2911,7 +2944,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>124</v>
       </c>
@@ -2934,7 +2967,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>124</v>
       </c>
@@ -2957,7 +2990,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>650</v>
       </c>
@@ -2980,7 +3013,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>650</v>
       </c>
@@ -3003,7 +3036,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>99</v>
       </c>
@@ -3026,7 +3059,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>99</v>
       </c>
@@ -3049,7 +3082,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>99</v>
       </c>
@@ -3072,7 +3105,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>353</v>
       </c>
@@ -3095,7 +3128,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>353</v>
       </c>
@@ -3118,7 +3151,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>353</v>
       </c>
@@ -3141,7 +3174,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>373</v>
       </c>
@@ -3164,7 +3197,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>373</v>
       </c>
@@ -3187,7 +3220,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>694</v>
       </c>
@@ -3210,7 +3243,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>694</v>
       </c>
@@ -3233,7 +3266,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>699</v>
       </c>
@@ -3256,7 +3289,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>133</v>
       </c>
@@ -3279,7 +3312,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>133</v>
       </c>
@@ -3302,7 +3335,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>364</v>
       </c>
@@ -3325,7 +3358,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>364</v>
       </c>
@@ -3348,7 +3381,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>565</v>
       </c>
@@ -3371,7 +3404,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>304</v>
       </c>
@@ -3394,7 +3427,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>304</v>
       </c>
@@ -3417,7 +3450,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>304</v>
       </c>
@@ -3440,7 +3473,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>277</v>
       </c>
@@ -3463,7 +3496,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>496</v>
       </c>
@@ -3486,7 +3519,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>398</v>
       </c>
@@ -3509,7 +3542,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>398</v>
       </c>
@@ -3532,7 +3565,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>398</v>
       </c>
@@ -3555,7 +3588,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>68</v>
       </c>
@@ -3578,7 +3611,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>68</v>
       </c>
@@ -3601,7 +3634,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>359</v>
       </c>
@@ -3624,7 +3657,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>359</v>
       </c>
@@ -3647,7 +3680,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>558</v>
       </c>
@@ -3670,7 +3703,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>150</v>
       </c>
@@ -3693,7 +3726,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>641</v>
       </c>
@@ -3716,7 +3749,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>176</v>
       </c>
@@ -3739,7 +3772,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>176</v>
       </c>
@@ -3762,7 +3795,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>176</v>
       </c>
@@ -3785,7 +3818,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>159</v>
       </c>
@@ -3808,7 +3841,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>434</v>
       </c>
@@ -3831,7 +3864,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
@@ -3854,7 +3887,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>438</v>
       </c>
@@ -3877,7 +3910,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>438</v>
       </c>
@@ -3900,7 +3933,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>146</v>
       </c>
@@ -3923,7 +3956,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>720</v>
       </c>
@@ -3946,7 +3979,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>243</v>
       </c>
@@ -3969,7 +4002,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>41</v>
       </c>
@@ -3992,7 +4025,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>41</v>
       </c>
@@ -4015,7 +4048,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>477</v>
       </c>
@@ -4038,7 +4071,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>412</v>
       </c>
@@ -4061,7 +4094,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>412</v>
       </c>
@@ -4084,7 +4117,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>711</v>
       </c>
@@ -4107,7 +4140,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>711</v>
       </c>
@@ -4130,7 +4163,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>218</v>
       </c>
@@ -4153,7 +4186,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>667</v>
       </c>
@@ -4176,7 +4209,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>667</v>
       </c>
@@ -4199,7 +4232,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>536</v>
       </c>
@@ -4222,7 +4255,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>606</v>
       </c>
@@ -4245,7 +4278,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>488</v>
       </c>
@@ -4268,7 +4301,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>488</v>
       </c>
@@ -4291,7 +4324,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>382</v>
       </c>
@@ -4314,7 +4347,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>7</v>
       </c>
@@ -4337,7 +4370,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>581</v>
       </c>
@@ -4360,7 +4393,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>324</v>
       </c>
@@ -4383,7 +4416,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>654</v>
       </c>
@@ -4406,7 +4439,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>654</v>
       </c>
@@ -4429,7 +4462,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>284</v>
       </c>
@@ -4452,7 +4485,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>723</v>
       </c>
@@ -4475,7 +4508,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>723</v>
       </c>
@@ -4498,7 +4531,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>191</v>
       </c>
@@ -4521,7 +4554,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>191</v>
       </c>
@@ -4544,7 +4577,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>500</v>
       </c>
@@ -4567,7 +4600,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>500</v>
       </c>
@@ -4590,7 +4623,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>292</v>
       </c>
@@ -4613,7 +4646,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>292</v>
       </c>
@@ -4636,7 +4669,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>292</v>
       </c>
@@ -4659,7 +4692,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>336</v>
       </c>
@@ -4682,7 +4715,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>532</v>
       </c>
@@ -4705,7 +4738,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>385</v>
       </c>
@@ -4728,7 +4761,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>473</v>
       </c>
@@ -4751,7 +4784,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>573</v>
       </c>
@@ -4774,7 +4807,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>269</v>
       </c>
@@ -4797,7 +4830,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>269</v>
       </c>
@@ -4820,7 +4853,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>269</v>
       </c>
@@ -4843,7 +4876,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>378</v>
       </c>
@@ -4866,7 +4899,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>671</v>
       </c>
@@ -4889,7 +4922,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>33</v>
       </c>
@@ -4912,7 +4945,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>33</v>
       </c>
@@ -4935,7 +4968,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>33</v>
       </c>
@@ -4958,7 +4991,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>186</v>
       </c>
@@ -4981,7 +5014,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>186</v>
       </c>
@@ -5004,7 +5037,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>645</v>
       </c>
@@ -5027,7 +5060,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>645</v>
       </c>
@@ -5050,7 +5083,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>645</v>
       </c>
@@ -5073,7 +5106,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>610</v>
       </c>
@@ -5096,7 +5129,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>610</v>
       </c>
@@ -5119,7 +5152,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
         <v>610</v>
       </c>
@@ -5142,7 +5175,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>470</v>
       </c>
@@ -5165,7 +5198,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
         <v>210</v>
       </c>
@@ -5188,7 +5221,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
         <v>251</v>
       </c>
@@ -5211,7 +5244,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
         <v>120</v>
       </c>
@@ -5234,7 +5267,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
         <v>421</v>
       </c>
@@ -5257,7 +5290,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>421</v>
       </c>
@@ -5280,7 +5313,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
         <v>222</v>
       </c>
@@ -5303,7 +5336,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
         <v>394</v>
       </c>
@@ -5326,7 +5359,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
         <v>522</v>
       </c>
@@ -5349,7 +5382,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
         <v>690</v>
       </c>
@@ -5372,7 +5405,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
         <v>315</v>
       </c>
@@ -5395,7 +5428,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
         <v>315</v>
       </c>
@@ -5418,7 +5451,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
         <v>543</v>
       </c>
@@ -5441,7 +5474,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
         <v>51</v>
       </c>
@@ -5464,7 +5497,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
         <v>288</v>
       </c>
@@ -5487,7 +5520,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
         <v>166</v>
       </c>
@@ -5510,7 +5543,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
         <v>214</v>
       </c>
@@ -5533,7 +5566,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
         <v>602</v>
       </c>
@@ -5556,7 +5589,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
         <v>417</v>
       </c>
@@ -5579,7 +5612,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
         <v>509</v>
       </c>
@@ -5602,7 +5635,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
         <v>686</v>
       </c>
@@ -5625,7 +5658,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
         <v>540</v>
       </c>
@@ -5648,7 +5681,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
         <v>46</v>
       </c>
@@ -5671,7 +5704,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
         <v>46</v>
       </c>
@@ -5694,7 +5727,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
         <v>369</v>
       </c>
@@ -5717,7 +5750,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
         <v>320</v>
       </c>
@@ -5740,7 +5773,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
         <v>202</v>
       </c>
@@ -5763,7 +5796,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
         <v>83</v>
       </c>
@@ -5786,7 +5819,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
         <v>83</v>
       </c>
@@ -5809,7 +5842,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
         <v>83</v>
       </c>
@@ -5832,7 +5865,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
         <v>596</v>
       </c>
@@ -5855,7 +5888,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
         <v>453</v>
       </c>
@@ -5878,7 +5911,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
         <v>116</v>
       </c>
@@ -5901,7 +5934,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
         <v>480</v>
       </c>
@@ -5924,7 +5957,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
         <v>547</v>
       </c>
@@ -5947,7 +5980,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
         <v>62</v>
       </c>
@@ -5970,7 +6003,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
         <v>62</v>
       </c>
@@ -5993,7 +6026,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
         <v>577</v>
       </c>
@@ -6016,7 +6049,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
         <v>404</v>
       </c>
@@ -6039,7 +6072,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
         <v>239</v>
       </c>
@@ -6062,7 +6095,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
         <v>13</v>
       </c>
@@ -6085,7 +6118,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>13</v>
       </c>
@@ -6108,7 +6141,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
         <v>138</v>
       </c>
@@ -6131,7 +6164,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
         <v>585</v>
       </c>
@@ -6154,7 +6187,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
         <v>585</v>
       </c>
@@ -6177,7 +6210,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
         <v>300</v>
       </c>
@@ -6200,7 +6233,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
         <v>562</v>
       </c>
@@ -6223,7 +6256,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
         <v>112</v>
       </c>
@@ -6246,7 +6279,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
         <v>592</v>
       </c>
@@ -6269,7 +6302,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
         <v>20</v>
       </c>
@@ -6292,7 +6325,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
         <v>616</v>
       </c>
@@ -6315,7 +6348,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
         <v>206</v>
       </c>
@@ -6338,7 +6371,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
         <v>551</v>
       </c>
@@ -6361,7 +6394,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
         <v>297</v>
       </c>
@@ -6384,7 +6417,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
         <v>297</v>
       </c>
@@ -6407,7 +6440,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
         <v>513</v>
       </c>
@@ -6430,7 +6463,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
         <v>513</v>
       </c>
@@ -6453,7 +6486,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
         <v>88</v>
       </c>
@@ -6476,7 +6509,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
         <v>88</v>
       </c>
@@ -6499,7 +6532,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
         <v>88</v>
       </c>
@@ -6522,7 +6555,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
         <v>675</v>
       </c>
@@ -6545,7 +6578,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
         <v>675</v>
       </c>
@@ -6568,7 +6601,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
         <v>675</v>
       </c>
@@ -6591,7 +6624,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A176" s="1" t="s">
         <v>430</v>
       </c>
@@ -6614,7 +6647,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
         <v>554</v>
       </c>
@@ -6637,7 +6670,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
         <v>182</v>
       </c>
@@ -6660,7 +6693,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A179" s="1" t="s">
         <v>658</v>
       </c>
@@ -6683,7 +6716,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A180" s="1" t="s">
         <v>658</v>
       </c>
@@ -6706,7 +6739,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A181" s="1" t="s">
         <v>170</v>
       </c>
@@ -6729,7 +6762,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A182" s="1" t="s">
         <v>170</v>
       </c>
@@ -6752,7 +6785,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A183" s="1" t="s">
         <v>170</v>
       </c>
@@ -6775,7 +6808,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A184" s="1" t="s">
         <v>344</v>
       </c>
@@ -6798,7 +6831,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A185" s="1" t="s">
         <v>344</v>
       </c>
@@ -6821,7 +6854,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="s">
         <v>448</v>
       </c>
@@ -6844,7 +6877,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A187" s="1" t="s">
         <v>448</v>
       </c>
@@ -6867,7 +6900,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A188" s="1" t="s">
         <v>448</v>
       </c>
@@ -6890,7 +6923,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A189" s="1" t="s">
         <v>569</v>
       </c>
@@ -6913,7 +6946,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A190" s="1" t="s">
         <v>78</v>
       </c>
@@ -6936,7 +6969,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A191" s="1" t="s">
         <v>78</v>
       </c>
@@ -6959,7 +6992,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A192" s="1" t="s">
         <v>599</v>
       </c>
@@ -6982,7 +7015,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A193" s="1" t="s">
         <v>310</v>
       </c>
@@ -7005,7 +7038,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A194" s="1" t="s">
         <v>310</v>
       </c>
@@ -7028,7 +7061,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A195" s="1" t="s">
         <v>332</v>
       </c>
@@ -7051,7 +7084,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A196" s="1" t="s">
         <v>196</v>
       </c>
@@ -7074,7 +7107,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A197" s="1" t="s">
         <v>196</v>
       </c>
@@ -7097,7 +7130,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A198" s="1" t="s">
         <v>457</v>
       </c>
@@ -7120,7 +7153,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A199" s="1" t="s">
         <v>457</v>
       </c>
@@ -7143,7 +7176,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A200" s="1" t="s">
         <v>106</v>
       </c>
@@ -7166,7 +7199,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A201" s="1" t="s">
         <v>106</v>
       </c>
@@ -7189,7 +7222,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A202" s="1" t="s">
         <v>633</v>
       </c>
@@ -7212,7 +7245,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A203" s="1" t="s">
         <v>461</v>
       </c>
@@ -7235,7 +7268,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A204" s="1" t="s">
         <v>663</v>
       </c>
@@ -7258,7 +7291,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A205" s="1" t="s">
         <v>663</v>
       </c>
@@ -7281,7 +7314,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A206" s="1" t="s">
         <v>58</v>
       </c>
@@ -7304,7 +7337,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A207" s="1" t="s">
         <v>389</v>
       </c>
@@ -7327,7 +7360,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A208" s="1" t="s">
         <v>389</v>
       </c>
@@ -7350,7 +7383,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A209" s="1" t="s">
         <v>389</v>
       </c>
@@ -7373,7 +7406,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A210" s="1" t="s">
         <v>703</v>
       </c>
@@ -7396,7 +7429,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A211" s="1" t="s">
         <v>637</v>
       </c>
@@ -7419,7 +7452,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A212" s="1" t="s">
         <v>637</v>
       </c>
@@ -7442,7 +7475,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A213" s="1" t="s">
         <v>637</v>
       </c>
@@ -7465,7 +7498,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A214" s="1" t="s">
         <v>281</v>
       </c>
@@ -7488,7 +7521,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A215" s="1" t="s">
         <v>129</v>
       </c>
@@ -7511,7 +7544,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A216" s="1" t="s">
         <v>518</v>
       </c>
@@ -7534,7 +7567,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A217" s="1" t="s">
         <v>518</v>
       </c>
@@ -7557,7 +7590,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A218" s="1" t="s">
         <v>707</v>
       </c>
@@ -7580,7 +7613,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A219" s="1" t="s">
         <v>707</v>
       </c>
@@ -7603,7 +7636,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A220" s="1" t="s">
         <v>464</v>
       </c>
@@ -7626,7 +7659,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A221" s="1" t="s">
         <v>464</v>
       </c>
@@ -7649,7 +7682,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A222" s="1" t="s">
         <v>426</v>
       </c>
@@ -7672,7 +7705,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A223" s="1" t="s">
         <v>255</v>
       </c>
@@ -7695,7 +7728,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A224" s="1" t="s">
         <v>247</v>
       </c>
@@ -7718,7 +7751,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A225" s="1" t="s">
         <v>589</v>
       </c>
@@ -7741,7 +7774,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A226" s="1" t="s">
         <v>230</v>
       </c>
@@ -7764,7 +7797,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A227" s="1" t="s">
         <v>526</v>
       </c>
@@ -7787,7 +7820,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A228" s="1" t="s">
         <v>526</v>
       </c>
@@ -7810,7 +7843,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A229" s="1" t="s">
         <v>526</v>
       </c>
@@ -7833,7 +7866,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A230" s="1" t="s">
         <v>154</v>
       </c>
@@ -7856,7 +7889,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A231" s="1" t="s">
         <v>154</v>
       </c>
@@ -7879,7 +7912,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A232" s="1" t="s">
         <v>259</v>
       </c>
@@ -7902,7 +7935,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A233" s="1" t="s">
         <v>259</v>
       </c>
@@ -7925,7 +7958,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A234" s="1" t="s">
         <v>259</v>
       </c>
@@ -7948,7 +7981,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A235" s="1" t="s">
         <v>620</v>
       </c>
@@ -7971,7 +8004,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A236" s="1" t="s">
         <v>620</v>
       </c>
@@ -7994,7 +8027,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A237" s="1" t="s">
         <v>234</v>
       </c>
@@ -8017,7 +8050,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A238" s="1" t="s">
         <v>234</v>
       </c>
@@ -8040,7 +8073,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A239" s="1" t="s">
         <v>728</v>
       </c>
@@ -8063,7 +8096,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A240" s="1" t="s">
         <v>728</v>
       </c>
@@ -8086,7 +8119,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A241" s="1" t="s">
         <v>73</v>
       </c>
@@ -8109,7 +8142,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A242" s="1" t="s">
         <v>73</v>
       </c>
@@ -8132,7 +8165,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A243" s="1" t="s">
         <v>339</v>
       </c>
@@ -8155,7 +8188,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A244" s="1" t="s">
         <v>339</v>
       </c>
@@ -8178,7 +8211,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A245" s="1" t="s">
         <v>339</v>
       </c>
@@ -8201,7 +8234,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A246" s="1" t="s">
         <v>25</v>
       </c>
@@ -8224,7 +8257,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A247" s="1" t="s">
         <v>25</v>
       </c>
@@ -8247,7 +8280,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A248" s="1" t="s">
         <v>25</v>
       </c>
@@ -8270,7 +8303,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A249" s="1" t="s">
         <v>625</v>
       </c>
@@ -8293,7 +8326,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A250" s="1" t="s">
         <v>625</v>
       </c>
@@ -8316,7 +8349,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A251" s="1" t="s">
         <v>504</v>
       </c>
@@ -8339,7 +8372,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A252" s="1" t="s">
         <v>504</v>
       </c>
@@ -8362,7 +8395,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A253" s="1" t="s">
         <v>408</v>
       </c>
@@ -8385,7 +8418,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A254" s="1" t="s">
         <v>408</v>
       </c>
@@ -8408,7 +8441,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A255" s="1" t="s">
         <v>484</v>
       </c>
@@ -8431,7 +8464,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A256" s="1" t="s">
         <v>484</v>
       </c>
@@ -8454,7 +8487,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A257" s="1" t="s">
         <v>94</v>
       </c>
@@ -8477,7 +8510,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A258" s="1" t="s">
         <v>94</v>
       </c>
@@ -8500,7 +8533,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A259" s="1" t="s">
         <v>226</v>
       </c>
@@ -8523,7 +8556,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A260" s="1" t="s">
         <v>492</v>
       </c>
@@ -8546,7 +8579,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A261" s="1" t="s">
         <v>492</v>
       </c>
@@ -8569,7 +8602,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A262" s="1" t="s">
         <v>327</v>
       </c>
@@ -8592,7 +8625,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A263" s="1" t="s">
         <v>327</v>
       </c>
@@ -8613,6 +8646,34 @@
       </c>
       <c r="G263" s="1" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A264" s="4" t="s">
+        <v>733</v>
+      </c>
+      <c r="B264" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="C264" s="4" t="s">
+        <v>735</v>
+      </c>
+      <c r="D264" s="3">
+        <v>214.26400000000001</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A265" s="5" t="s">
+        <v>736</v>
+      </c>
+      <c r="B265" s="4" t="s">
+        <v>737</v>
+      </c>
+      <c r="C265" s="4" t="s">
+        <v>738</v>
+      </c>
+      <c r="D265" s="1">
+        <v>268.35599999999999</v>
       </c>
     </row>
   </sheetData>
@@ -8625,6 +8686,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010058B55FF886ACD04FA46F351C1187A9BD" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d91ccc915f7c5179be56c7753de5fad7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="198292a3-4908-4712-b2cc-f3b3658c84fe" xmlns:ns3="e0a953a8-67bd-452e-b19a-3db8bd21fe50" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a9c20e60bd321f5cd18176ed7d20cc2" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -8916,15 +8986,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -8946,13 +9007,41 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27493AB9-CA62-43F5-96D9-CACB635D311D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87736FEB-0BDC-4DB5-B55B-29D37DC4E0DA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87736FEB-0BDC-4DB5-B55B-29D37DC4E0DA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27493AB9-CA62-43F5-96D9-CACB635D311D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="198292a3-4908-4712-b2cc-f3b3658c84fe"/>
+    <ds:schemaRef ds:uri="e0a953a8-67bd-452e-b19a-3db8bd21fe50"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9EB35607-6B78-4CFD-8E92-81B825D290F4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9EB35607-6B78-4CFD-8E92-81B825D290F4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="198292a3-4908-4712-b2cc-f3b3658c84fe"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="e0a953a8-67bd-452e-b19a-3db8bd21fe50"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>